<commit_message>
PROS-11269 - CCRU - PoS update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/Benchmark 2019.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/Benchmark 2019.xlsx
@@ -1,34 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My folder\RED\POS\POS_20190723_1938\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64F33C2-6D8D-4D5F-9D55-B90F3A96D4BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="992" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Conv Big CAP" sheetId="1" r:id="rId1"/>
-    <sheet name="Conv Other" sheetId="2" r:id="rId2"/>
-    <sheet name="Hyper" sheetId="3" r:id="rId3"/>
-    <sheet name="Super CAP" sheetId="4" r:id="rId4"/>
-    <sheet name="Super REG" sheetId="5" r:id="rId5"/>
-    <sheet name="HoReCa" sheetId="6" r:id="rId6"/>
-    <sheet name="FastFood" sheetId="14" r:id="rId7"/>
-    <sheet name="QSR-Cinema" sheetId="7" r:id="rId8"/>
-    <sheet name="Petrol" sheetId="8" r:id="rId9"/>
-    <sheet name="Canteen EDU" sheetId="9" r:id="rId10"/>
-    <sheet name="Canteen OTH" sheetId="10" r:id="rId11"/>
-    <sheet name="FT" sheetId="11" r:id="rId12"/>
-    <sheet name="FT NS CAP" sheetId="12" r:id="rId13"/>
-    <sheet name="FT NS REG" sheetId="13" r:id="rId14"/>
+    <sheet name="Conv Big CAP" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Conv Other" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Hyper" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Super CAP" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Super REG" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="HoReCa" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="FastFood" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="QSR-Cinema" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Petrol" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Canteen EDU" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Canteen OTH" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="FT" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="FT NS CAP" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="FT NS REG" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -38,149 +33,149 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="64">
-  <si>
-    <t>KPI Code</t>
-  </si>
-  <si>
-    <t>KPI Name</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>Value Type</t>
-  </si>
-  <si>
-    <t>Values</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="62">
+  <si>
+    <t xml:space="preserve">KPI Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values</t>
   </si>
   <si>
     <t xml:space="preserve">STANDARD 1     </t>
   </si>
   <si>
-    <t>Number of SSD core assortment available in-store</t>
-  </si>
-  <si>
-    <t>POS KPI</t>
-  </si>
-  <si>
-    <t>SSD Availability</t>
+    <t xml:space="preserve">Number of SSD core assortment available in-store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS KPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Availability</t>
   </si>
   <si>
     <t xml:space="preserve">STANDARD 2   </t>
   </si>
   <si>
-    <t>Number of NCB core assortment available in-store</t>
-  </si>
-  <si>
-    <t>Water Availability,
+    <t xml:space="preserve">Number of NCB core assortment available in-store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Availability,
 Energy Availability,
 Tea Availability,
 Juice (JNSD) Availability</t>
   </si>
   <si>
-    <t>STANDARD 20</t>
-  </si>
-  <si>
-    <t>CCH shelf share in SSD</t>
-  </si>
-  <si>
-    <t>SSD Shelf: Shelf share</t>
+    <t xml:space="preserve">STANDARD 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH shelf share in SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Shelf: Shelf share</t>
   </si>
   <si>
     <t xml:space="preserve">STANDARD 21 </t>
   </si>
   <si>
-    <t>CCH shelf share in Water</t>
-  </si>
-  <si>
-    <t>Water Shelf: Shelf share</t>
+    <t xml:space="preserve">CCH shelf share in Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Shelf: Shelf share</t>
   </si>
   <si>
     <t xml:space="preserve">STANDARD 23 </t>
   </si>
   <si>
-    <t>CCH shelf share in Juice</t>
-  </si>
-  <si>
-    <t>Juice Shelf: Shelf share</t>
+    <t xml:space="preserve">CCH shelf share in Juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Shelf: Shelf share</t>
   </si>
   <si>
     <t xml:space="preserve">STANDARD 24  </t>
   </si>
   <si>
-    <t>CCH shelf share in Tea</t>
-  </si>
-  <si>
-    <t>Ice Tea Shelf: Shelf share</t>
+    <t xml:space="preserve">CCH shelf share in Tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Tea Shelf: Shelf share</t>
   </si>
   <si>
     <t xml:space="preserve">STANDARD 25  </t>
   </si>
   <si>
-    <t>CCH shelf share in Energy</t>
-  </si>
-  <si>
-    <t>Energy Shelf: Shelf share</t>
-  </si>
-  <si>
-    <t>STANDARD 27</t>
-  </si>
-  <si>
-    <t>Number of CCH displays points of interaction</t>
-  </si>
-  <si>
-    <t>SSD Display 1st,
+    <t xml:space="preserve">CCH shelf share in Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Shelf: Shelf share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of CCH displays points of interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 1st,
 Juice Display 1st,
 SSD Display 2d,
 NCB-Mixability Display</t>
   </si>
   <si>
-    <t>STANDARD 22</t>
-  </si>
-  <si>
-    <t>Number of CCH cooler doors and-or equivalent in Customer coolers</t>
-  </si>
-  <si>
-    <t>Cooler: Doors</t>
-  </si>
-  <si>
-    <t>STANDARD 18</t>
-  </si>
-  <si>
-    <t>CCH coolers quality</t>
-  </si>
-  <si>
-    <t>Cooler: Prime Position,
+    <t xml:space="preserve">STANDARD 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of CCH cooler doors and-or equivalent in Customer coolers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH coolers quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Prime Position,
 Cooler: Max 15,
 Cooler: Merch Priorty STD,
 Cooler: w/o other products</t>
   </si>
   <si>
-    <t>SSD Display 1st,
+    <t xml:space="preserve">SSD Display 1st,
 Juice Display 1st,
 SSD Display 2d</t>
   </si>
   <si>
-    <t>STANDARD 1</t>
-  </si>
-  <si>
-    <t>STANDARD 2</t>
-  </si>
-  <si>
-    <t>STANDARD 21</t>
-  </si>
-  <si>
-    <t>STANDARD 23</t>
-  </si>
-  <si>
-    <t>STANDARD 24</t>
-  </si>
-  <si>
-    <t>STANDARD 25</t>
-  </si>
-  <si>
-    <t>SSD Display 1st,
+    <t xml:space="preserve">STANDARD 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 1st,
 SSD Display 2d,
 Juice Display 2d,
 NCB Display,
@@ -191,7 +186,7 @@
 SSD Display 4th</t>
   </si>
   <si>
-    <t>SSD Display 1st,
+    <t xml:space="preserve">SSD Display 1st,
 Juice Display 1st,
 SSD Display 2d,
 NCB Display,
@@ -200,93 +195,100 @@
 Mixability Display</t>
   </si>
   <si>
-    <t>Juice Availability,
+    <t xml:space="preserve">Juice (JNSD) Availability,
 Energy Availability,
 Water Availability</t>
   </si>
   <si>
-    <t>STANDARD 16</t>
-  </si>
-  <si>
-    <t>CCH products present in Customers menu</t>
-  </si>
-  <si>
-    <t>Menu Activation</t>
-  </si>
-  <si>
-    <t>STANDARD 17</t>
-  </si>
-  <si>
-    <t>Number of CCH activation points in NARTD</t>
-  </si>
-  <si>
-    <t>Impulse Activation,
+    <t xml:space="preserve">STANDARD 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH products present in Customers menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of CCH activation points in NARTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulse Activation,
 Destination Activation</t>
   </si>
   <si>
-    <t>Water Availability,
-Energy Availability,
-Tea Availability,
-Juice Availability</t>
-  </si>
-  <si>
-    <t>Combo</t>
-  </si>
-  <si>
-    <t>Impulse Activation</t>
-  </si>
-  <si>
-    <t>Cooler: Prime Position,
+    <t xml:space="preserve">Combo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Prime Position,
 Cooler: w/o other products,
 Cooler: Max 15</t>
   </si>
   <si>
-    <t>Juice Availability,
+    <t xml:space="preserve">Impulse Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice (JNSD) Availability,
 Energy Availability,
 Water Availability,
 Tea Availability</t>
   </si>
   <si>
-    <t>Zone Activation Impulse/Cash,
+    <t xml:space="preserve">Zone Activation Impulse/Cash,
 Combo</t>
   </si>
   <si>
-    <t>Juice Availability,
+    <t xml:space="preserve">Juice (JNSD) Availability,
 Water Availability,
 Tea Availability</t>
   </si>
   <si>
-    <t>Activation bufet line,
+    <t xml:space="preserve">Activation bufet line,
 Combo</t>
   </si>
   <si>
-    <t>SSD Display,
+    <t xml:space="preserve">SSD Display,
 Juice Display</t>
   </si>
   <si>
-    <t>JNSD Displays</t>
-  </si>
-  <si>
-    <t>Juice Display</t>
-  </si>
-  <si>
-    <t>Menu activation</t>
+    <t xml:space="preserve">Juice Display</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -296,14 +298,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,73 +320,116 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+  <cellXfs count="12">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -429,7 +474,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF92D050"/>
       <rgbColor rgb="FFFFC000"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -443,341 +488,33 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -794,14 +531,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -811,14 +548,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -828,14 +565,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -845,14 +582,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -862,14 +599,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -879,14 +616,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -896,14 +633,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -913,14 +650,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -930,14 +667,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -947,14 +684,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -965,9 +702,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -975,24 +713,27 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMK6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1009,14 +750,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1.111111</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1026,31 +767,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1.111111</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1.111111</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1060,14 +801,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1.111111</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1077,27 +818,28 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>1.111111</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1105,24 +847,27 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:AMK6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1139,14 +884,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1.111111</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1156,31 +901,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1.111111</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1.111111</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1190,14 +935,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1.111111</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1207,27 +952,28 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>1.111111</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1235,24 +981,27 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:AMK6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1269,14 +1018,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1286,14 +1035,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1303,14 +1052,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1320,14 +1069,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1337,14 +1086,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1355,9 +1104,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1365,24 +1115,27 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:AMK6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1399,14 +1152,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1416,14 +1169,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1433,31 +1186,31 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1467,14 +1220,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1485,9 +1238,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1495,24 +1249,27 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:AMK6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1529,14 +1286,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1546,14 +1303,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1563,31 +1320,31 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1597,14 +1354,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1615,9 +1372,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1625,24 +1383,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1659,14 +1420,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1676,14 +1437,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1693,14 +1454,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1710,14 +1471,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1727,14 +1488,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1744,14 +1505,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1761,14 +1522,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1778,14 +1539,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1795,14 +1556,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1812,14 +1573,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="2" t="n">
         <v>1.123596</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1830,9 +1591,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1840,24 +1602,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1874,15 +1639,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C2" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -1891,15 +1656,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C3" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -1908,15 +1673,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C4" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -1925,15 +1690,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C5" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -1942,15 +1707,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C6" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -1959,15 +1724,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C7" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
@@ -1976,15 +1741,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C8" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>7</v>
@@ -1993,15 +1758,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C9" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
@@ -2010,15 +1775,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C10" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
@@ -2028,9 +1793,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2038,24 +1804,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2072,15 +1841,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C2" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -2089,15 +1858,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C3" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -2106,15 +1875,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C4" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -2123,15 +1892,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C5" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -2140,15 +1909,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C6" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -2157,15 +1926,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C7" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
@@ -2174,15 +1943,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C8" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>7</v>
@@ -2191,15 +1960,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C9" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
@@ -2208,15 +1977,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C10" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
@@ -2226,9 +1995,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2236,24 +2006,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AMK10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2270,15 +2043,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C2" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -2287,15 +2060,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C3" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -2304,15 +2077,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C4" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -2321,15 +2094,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C5" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -2338,15 +2111,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C6" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -2355,15 +2128,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C7" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
@@ -2372,15 +2145,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C8" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>7</v>
@@ -2389,15 +2162,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C9" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
@@ -2406,15 +2179,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2">
-        <v>1.1976047999999999</v>
+      <c r="C10" s="2" t="n">
+        <v>1.1976048</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
@@ -2424,9 +2197,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2434,24 +2208,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AMK5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2468,14 +2245,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1.200048</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2485,31 +2262,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1.200048</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1.200048</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2519,14 +2296,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1.200048</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -2537,9 +2314,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2547,24 +2325,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FECCAC62-317B-4118-BAAF-F7AB0A6489AD}">
-  <dimension ref="A1:AMK7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="1025" width="8.7265625" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="58.4858299595142"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="7.81781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2581,14 +2362,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2598,65 +2379,65 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -2666,27 +2447,28 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2694,24 +2476,27 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMK7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2728,14 +2513,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2745,65 +2530,65 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -2813,27 +2598,28 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="2" t="n">
         <v>1.38889</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2841,24 +2627,27 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMK9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="2" width="69.54296875" style="1"/>
-    <col min="3" max="3" width="10.08984375" style="2"/>
-    <col min="4" max="4" width="13.6328125" style="2"/>
-    <col min="5" max="5" width="38.26953125" style="1"/>
-    <col min="6" max="1025" width="8.54296875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2875,14 +2664,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2892,31 +2681,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2926,14 +2715,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -2943,14 +2732,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -2960,14 +2749,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2977,14 +2766,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -2994,27 +2783,28 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="2" t="n">
         <v>1.176471</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>